<commit_message>
Solución a tickets AID-369, AID-370 Y AID-413
</commit_message>
<xml_diff>
--- a/Diverscan.MJP.UI/temp/Inventario.xlsx
+++ b/Diverscan.MJP.UI/temp/Inventario.xlsx
@@ -5,13 +5,13 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="R63e90451e14b43fb"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="R13f3ecd7de7c4e2c"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Id Solicitud</t>
   </si>
@@ -37,28 +37,19 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>01-01-01</t>
+    <t>20301-00420-0240</t>
   </si>
   <si>
-    <t>Liquido Hidráulico frenos</t>
+    <t>CANDADO DE BRONCE DE 38 /40 MM</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>ml</t>
+    <t>GENERICO</t>
   </si>
   <si>
-    <t>(91)I_02-PIC-00A-001-001-001</t>
-  </si>
-  <si>
-    <t>01-01-11</t>
-  </si>
-  <si>
-    <t>Aceite motor HW40</t>
-  </si>
-  <si>
-    <t>(91)I_02-PIC-00A-001-001-002</t>
+    <t>(91)B09-PIC-00B-001-001-001</t>
   </si>
 </sst>
 </file>
@@ -104,20 +95,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.0949881417411" customWidth="1"/>
-    <col min="2" max="2" width="9.29643957955497" customWidth="1"/>
-    <col min="3" max="3" width="23.3574480329241" customWidth="1"/>
+    <col min="1" max="1" width="10.3633991588246" customWidth="1"/>
+    <col min="2" max="2" width="16.9981647838246" customWidth="1"/>
+    <col min="3" max="3" width="32.7081243341619" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.6317247663225" customWidth="1"/>
-    <col min="6" max="6" width="17.6252147129604" customWidth="1"/>
-    <col min="7" max="7" width="28.1085641043527" customWidth="1"/>
-    <col min="8" max="8" width="9.2493782043457" customWidth="1"/>
+    <col min="5" max="5" width="13.7393757213246" customWidth="1"/>
+    <col min="6" max="6" width="16.5967975963246" customWidth="1"/>
+    <col min="7" max="7" width="26.1065618341619" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -148,7 +139,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
@@ -169,33 +160,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0">
-        <v>2</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>